<commit_message>
feat : services created for all entities
</commit_message>
<xml_diff>
--- a/add-in.xlsx
+++ b/add-in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work-place\flutter apps\projects\sharp\BisleriumCafeBackend\BisleriumCafeBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5B8CA3-DDAD-46D1-ABFC-D395CC8515AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0025210A-A183-4A02-A440-E524B8FFBF3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Id</t>
   </si>
@@ -40,19 +40,10 @@
     <t>Price</t>
   </si>
   <si>
-    <t>sgdgf</t>
-  </si>
-  <si>
-    <t>Rohan</t>
-  </si>
-  <si>
     <t>chill</t>
   </si>
   <si>
-    <t>Sohan</t>
-  </si>
-  <si>
-    <t>fooking</t>
+    <t>shit</t>
   </si>
 </sst>
 </file>
@@ -60,18 +51,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -85,7 +68,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -93,26 +76,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" applyNumberFormat="0" fontId="1" applyFont="1" fillId="0" applyFill="0" borderId="1" applyBorder="1" applyProtection="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -391,10 +362,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,14 +374,14 @@
     <col min="2" max="2" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.8">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -433,40 +404,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="0">
-        <v>535.6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="0">
-        <v>3</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="0">
-        <v>535.6</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0">
-        <v>4</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="0">
-        <v>535.6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0">
-        <v>5</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="0">
-        <v>535.6</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat : starting working on order + member + coffee + addin
</commit_message>
<xml_diff>
--- a/add-in.xlsx
+++ b/add-in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work-place\flutter apps\projects\sharp\BisleriumCafeBackend\BisleriumCafeBackend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0025210A-A183-4A02-A440-E524B8FFBF3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDC74A6-4D7A-4E65-B0D4-3B0CE8F5A84D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Id</t>
   </si>
@@ -40,10 +40,7 @@
     <t>Price</t>
   </si>
   <si>
-    <t>chill</t>
-  </si>
-  <si>
-    <t>shit</t>
+    <t>vanilla</t>
   </si>
 </sst>
 </file>
@@ -362,16 +359,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -393,18 +391,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="0">
-        <v>535.6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="0">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="0">
-        <v>300</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat : temp attachment save complete
</commit_message>
<xml_diff>
--- a/add-in.xlsx
+++ b/add-in.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Id</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>vanilla</t>
+  </si>
+  <si>
+    <t>ICe Cream</t>
+  </si>
+  <si>
+    <t>straw</t>
   </si>
 </sst>
 </file>
@@ -359,7 +365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -394,6 +400,28 @@
         <v>200</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="0">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>